<commit_message>
Upload the final version of V5
</commit_message>
<xml_diff>
--- a/FN312_Dashboard_Outline_V5.xlsx
+++ b/FN312_Dashboard_Outline_V5.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" firstSheet="3" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="Home" sheetId="1" r:id="rId1"/>
@@ -9828,7 +9828,7 @@
   </sheetPr>
   <dimension ref="A1:P125"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
@@ -25497,8 +25497,8 @@
   </sheetPr>
   <dimension ref="A1:W44"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="P29" sqref="P29"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -25576,8 +25576,8 @@
         <v>195</v>
       </c>
       <c r="G3" s="89">
-        <f>DATE(2020, 9, 25)</f>
-        <v>44099</v>
+        <f>DATE(2020, 9, 24)</f>
+        <v>44098</v>
       </c>
       <c r="H3" s="68"/>
       <c r="I3" s="85"/>
@@ -28620,8 +28620,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S55"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32294,7 +32294,7 @@
   <dimension ref="A1:Y16"/>
   <sheetViews>
     <sheetView topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="Y4" sqref="Y4"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>